<commit_message>
day 3 oops program
</commit_message>
<xml_diff>
--- a/DAY 1/AJAY K_test_cast_design_for_redif_account_creation.xlsx
+++ b/DAY 1/AJAY K_test_cast_design_for_redif_account_creation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\HCL TRAINING ASSINGMENT\DAY 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1713,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7104,6 +7104,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100942A5F91C020114B9D9B6669BDED9868" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="62496d86c6ae077114fd1d88c4539805">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="24503b2e-f4dc-4abf-83fe-5a97c0785769" xmlns:ns3="e79f15d7-c448-4303-9ba2-b2daf1085145" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="22ddc5b4a67293e3563182d9cb923a11" ns2:_="" ns3:_="">
     <xsd:import namespace="24503b2e-f4dc-4abf-83fe-5a97c0785769"/>
@@ -7320,36 +7335,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E86B9FAD-4AF9-4744-AA50-00A254F1E863}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0CD53BC-1D15-4B9F-8123-00188531DB3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="24503b2e-f4dc-4abf-83fe-5a97c0785769"/>
-    <ds:schemaRef ds:uri="e79f15d7-c448-4303-9ba2-b2daf1085145"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7372,9 +7361,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0CD53BC-1D15-4B9F-8123-00188531DB3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E86B9FAD-4AF9-4744-AA50-00A254F1E863}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="24503b2e-f4dc-4abf-83fe-5a97c0785769"/>
+    <ds:schemaRef ds:uri="e79f15d7-c448-4303-9ba2-b2daf1085145"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>